<commit_message>
modell was split into import and analysis
</commit_message>
<xml_diff>
--- a/data/Technische Daten Gaskraftwerke.xlsx
+++ b/data/Technische Daten Gaskraftwerke.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="43" documentId="A09C9C68B51071510B526651E7DADA88F61A921B" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{48067E1D-9904-48AE-9ED4-672EE45A9DCC}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="A3111276CDCCE9161FC814EBDF092382908FD777" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{CE2535E3-E66E-4045-8516-E48E3B6166DC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GuD Kraftwerk" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
   <si>
     <t>Gas- und Dampfkraftwerk: Technische Daten</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>wert</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>marginal_cost</t>
   </si>
 </sst>
 </file>
@@ -661,7 +667,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,7 +729,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="7">
-        <v>595</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -797,11 +803,25 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="9"/>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -1007,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E53051-53FC-4C47-B45D-28B27563BB55}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1096,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="7">
-        <v>187</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1150,11 +1170,25 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="9"/>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
working exept for wind data
</commit_message>
<xml_diff>
--- a/data/Technische Daten Gaskraftwerke.xlsx
+++ b/data/Technische Daten Gaskraftwerke.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="A3111276CDCCE9161FC814EBDF092382908FD777" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{CE2535E3-E66E-4045-8516-E48E3B6166DC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="A3111276CDCCE9161FC814EBDF092382908FD777" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{4D9E171E-A98A-46BA-9826-D291E7706A3C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GuD Kraftwerk" sheetId="1" r:id="rId1"/>
@@ -666,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E53051-53FC-4C47-B45D-28B27563BB55}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1175,7 @@
         <v>79</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>